<commit_message>
finished 60001 asset allocation, and liquidity report, check README.md
</commit_message>
<xml_diff>
--- a/reports/BlpData_20201231.xlsx
+++ b/reports/BlpData_20201231.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhangst\git\risk_report\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD6802AC-5EA4-40BF-8427-EB23718AA074}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E2C8D7-508F-4FEA-9BC7-6738A9D8C585}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8FF2902-90D0-475C-A000-781CB7C08180}"/>
+    <workbookView xWindow="2688" yWindow="336" windowWidth="18264" windowHeight="12624" xr2:uid="{F8FF2902-90D0-475C-A000-781CB7C08180}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2268" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2316" uniqueCount="281">
   <si>
     <t>ID</t>
   </si>
@@ -868,6 +868,15 @@
   </si>
   <si>
     <t>XS1852561031</t>
+  </si>
+  <si>
+    <t>XS0852986156</t>
+  </si>
+  <si>
+    <t>XS1125272143</t>
+  </si>
+  <si>
+    <t>XS2008566197</t>
   </si>
 </sst>
 </file>
@@ -1219,15 +1228,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EC1C060-C25A-42A1-8D23-BCFA1068E096}">
-  <dimension ref="A1:L189"/>
+  <dimension ref="A1:L193"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="M187" sqref="M187"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1265,7 +1274,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1303,7 +1312,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1341,7 +1350,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1379,7 +1388,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1417,7 +1426,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1455,7 +1464,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -1493,7 +1502,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1531,7 +1540,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -1569,7 +1578,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -1607,7 +1616,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -1645,7 +1654,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -1683,7 +1692,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -1721,7 +1730,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -1759,7 +1768,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -1797,7 +1806,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -1835,7 +1844,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>62</v>
       </c>
@@ -1873,7 +1882,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>64</v>
       </c>
@@ -1911,7 +1920,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>66</v>
       </c>
@@ -1949,7 +1958,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>70</v>
       </c>
@@ -1987,7 +1996,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>71</v>
       </c>
@@ -2025,7 +2034,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>73</v>
       </c>
@@ -2063,7 +2072,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>76</v>
       </c>
@@ -2101,7 +2110,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>77</v>
       </c>
@@ -2139,7 +2148,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>78</v>
       </c>
@@ -2177,7 +2186,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>79</v>
       </c>
@@ -2215,7 +2224,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>81</v>
       </c>
@@ -2253,7 +2262,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>86</v>
       </c>
@@ -2291,7 +2300,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>88</v>
       </c>
@@ -2329,7 +2338,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>89</v>
       </c>
@@ -2367,7 +2376,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>92</v>
       </c>
@@ -2405,7 +2414,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>94</v>
       </c>
@@ -2443,7 +2452,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>95</v>
       </c>
@@ -2481,7 +2490,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>98</v>
       </c>
@@ -2519,7 +2528,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>99</v>
       </c>
@@ -2557,7 +2566,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>102</v>
       </c>
@@ -2595,7 +2604,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>103</v>
       </c>
@@ -2633,7 +2642,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>104</v>
       </c>
@@ -2671,7 +2680,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>105</v>
       </c>
@@ -2709,7 +2718,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>107</v>
       </c>
@@ -2747,7 +2756,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>108</v>
       </c>
@@ -2785,7 +2794,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>109</v>
       </c>
@@ -2823,7 +2832,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>112</v>
       </c>
@@ -2861,7 +2870,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>113</v>
       </c>
@@ -2899,7 +2908,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>114</v>
       </c>
@@ -2937,7 +2946,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>115</v>
       </c>
@@ -2975,7 +2984,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>117</v>
       </c>
@@ -3013,7 +3022,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>118</v>
       </c>
@@ -3051,7 +3060,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>120</v>
       </c>
@@ -3089,7 +3098,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>121</v>
       </c>
@@ -3127,7 +3136,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>122</v>
       </c>
@@ -3165,7 +3174,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>123</v>
       </c>
@@ -3203,7 +3212,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>124</v>
       </c>
@@ -3241,7 +3250,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>125</v>
       </c>
@@ -3279,7 +3288,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>126</v>
       </c>
@@ -3317,7 +3326,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>127</v>
       </c>
@@ -3355,7 +3364,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>128</v>
       </c>
@@ -3393,7 +3402,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>130</v>
       </c>
@@ -3431,7 +3440,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>131</v>
       </c>
@@ -3469,7 +3478,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>132</v>
       </c>
@@ -3507,7 +3516,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>133</v>
       </c>
@@ -3545,7 +3554,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>134</v>
       </c>
@@ -3583,7 +3592,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>135</v>
       </c>
@@ -3621,7 +3630,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>136</v>
       </c>
@@ -3659,7 +3668,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>137</v>
       </c>
@@ -3697,7 +3706,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>138</v>
       </c>
@@ -3735,7 +3744,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>140</v>
       </c>
@@ -3773,7 +3782,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>141</v>
       </c>
@@ -3811,7 +3820,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>142</v>
       </c>
@@ -3849,7 +3858,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>143</v>
       </c>
@@ -3887,7 +3896,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>144</v>
       </c>
@@ -3925,7 +3934,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>146</v>
       </c>
@@ -3963,7 +3972,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>151</v>
       </c>
@@ -4001,7 +4010,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>152</v>
       </c>
@@ -4039,7 +4048,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>153</v>
       </c>
@@ -4077,7 +4086,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>154</v>
       </c>
@@ -4115,7 +4124,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>155</v>
       </c>
@@ -4153,7 +4162,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>156</v>
       </c>
@@ -4191,7 +4200,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>158</v>
       </c>
@@ -4229,7 +4238,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>159</v>
       </c>
@@ -4267,7 +4276,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>160</v>
       </c>
@@ -4305,7 +4314,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>161</v>
       </c>
@@ -4343,7 +4352,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>162</v>
       </c>
@@ -4381,7 +4390,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>164</v>
       </c>
@@ -4419,7 +4428,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>165</v>
       </c>
@@ -4457,7 +4466,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>167</v>
       </c>
@@ -4495,7 +4504,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>168</v>
       </c>
@@ -4533,7 +4542,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>170</v>
       </c>
@@ -4571,7 +4580,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>171</v>
       </c>
@@ -4609,7 +4618,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>172</v>
       </c>
@@ -4647,7 +4656,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>173</v>
       </c>
@@ -4685,7 +4694,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>174</v>
       </c>
@@ -4723,7 +4732,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>175</v>
       </c>
@@ -4761,7 +4770,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>176</v>
       </c>
@@ -4799,7 +4808,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>178</v>
       </c>
@@ -4837,7 +4846,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>179</v>
       </c>
@@ -4875,7 +4884,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>180</v>
       </c>
@@ -4913,7 +4922,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>181</v>
       </c>
@@ -4951,7 +4960,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>182</v>
       </c>
@@ -4989,7 +4998,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>183</v>
       </c>
@@ -5027,7 +5036,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>184</v>
       </c>
@@ -5065,7 +5074,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>185</v>
       </c>
@@ -5103,7 +5112,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>186</v>
       </c>
@@ -5141,7 +5150,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>187</v>
       </c>
@@ -5179,7 +5188,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>188</v>
       </c>
@@ -5217,7 +5226,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>189</v>
       </c>
@@ -5255,7 +5264,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>190</v>
       </c>
@@ -5293,7 +5302,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>191</v>
       </c>
@@ -5331,7 +5340,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>192</v>
       </c>
@@ -5369,7 +5378,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>193</v>
       </c>
@@ -5407,7 +5416,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>194</v>
       </c>
@@ -5445,7 +5454,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>195</v>
       </c>
@@ -5483,7 +5492,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>196</v>
       </c>
@@ -5521,7 +5530,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>197</v>
       </c>
@@ -5559,7 +5568,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>198</v>
       </c>
@@ -5597,7 +5606,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>199</v>
       </c>
@@ -5635,7 +5644,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>200</v>
       </c>
@@ -5673,7 +5682,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>201</v>
       </c>
@@ -5711,7 +5720,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>202</v>
       </c>
@@ -5749,7 +5758,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>203</v>
       </c>
@@ -5787,7 +5796,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>204</v>
       </c>
@@ -5825,7 +5834,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>205</v>
       </c>
@@ -5863,7 +5872,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>206</v>
       </c>
@@ -5901,7 +5910,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>207</v>
       </c>
@@ -5939,7 +5948,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>208</v>
       </c>
@@ -5977,7 +5986,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>209</v>
       </c>
@@ -6015,7 +6024,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>210</v>
       </c>
@@ -6053,7 +6062,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>211</v>
       </c>
@@ -6091,7 +6100,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>212</v>
       </c>
@@ -6129,7 +6138,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>213</v>
       </c>
@@ -6167,7 +6176,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>214</v>
       </c>
@@ -6205,7 +6214,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>215</v>
       </c>
@@ -6243,7 +6252,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>216</v>
       </c>
@@ -6281,7 +6290,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>217</v>
       </c>
@@ -6319,7 +6328,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>218</v>
       </c>
@@ -6357,7 +6366,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>219</v>
       </c>
@@ -6395,7 +6404,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>221</v>
       </c>
@@ -6433,7 +6442,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>222</v>
       </c>
@@ -6471,7 +6480,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>223</v>
       </c>
@@ -6509,7 +6518,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>224</v>
       </c>
@@ -6547,7 +6556,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>225</v>
       </c>
@@ -6585,7 +6594,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>226</v>
       </c>
@@ -6623,7 +6632,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>227</v>
       </c>
@@ -6661,7 +6670,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>228</v>
       </c>
@@ -6699,7 +6708,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>229</v>
       </c>
@@ -6737,7 +6746,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>230</v>
       </c>
@@ -6775,7 +6784,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>231</v>
       </c>
@@ -6813,7 +6822,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>232</v>
       </c>
@@ -6851,7 +6860,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>233</v>
       </c>
@@ -6889,7 +6898,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>234</v>
       </c>
@@ -6927,7 +6936,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>235</v>
       </c>
@@ -6965,7 +6974,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>236</v>
       </c>
@@ -7003,7 +7012,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>240</v>
       </c>
@@ -7041,7 +7050,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>241</v>
       </c>
@@ -7079,7 +7088,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>242</v>
       </c>
@@ -7117,7 +7126,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>243</v>
       </c>
@@ -7155,7 +7164,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>244</v>
       </c>
@@ -7193,7 +7202,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>245</v>
       </c>
@@ -7231,7 +7240,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>246</v>
       </c>
@@ -7269,7 +7278,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>247</v>
       </c>
@@ -7307,7 +7316,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>248</v>
       </c>
@@ -7345,7 +7354,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>249</v>
       </c>
@@ -7383,7 +7392,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>250</v>
       </c>
@@ -7421,7 +7430,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>251</v>
       </c>
@@ -7459,7 +7468,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>252</v>
       </c>
@@ -7497,7 +7506,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>253</v>
       </c>
@@ -7535,7 +7544,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>254</v>
       </c>
@@ -7573,7 +7582,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>255</v>
       </c>
@@ -7611,7 +7620,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>257</v>
       </c>
@@ -7649,7 +7658,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>258</v>
       </c>
@@ -7687,7 +7696,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>259</v>
       </c>
@@ -7725,7 +7734,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>260</v>
       </c>
@@ -7763,7 +7772,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>261</v>
       </c>
@@ -7801,7 +7810,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>262</v>
       </c>
@@ -7839,7 +7848,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>263</v>
       </c>
@@ -7877,7 +7886,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>264</v>
       </c>
@@ -7915,7 +7924,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>265</v>
       </c>
@@ -7953,7 +7962,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>266</v>
       </c>
@@ -7991,7 +8000,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>267</v>
       </c>
@@ -8029,7 +8038,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>268</v>
       </c>
@@ -8067,7 +8076,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>269</v>
       </c>
@@ -8105,7 +8114,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>270</v>
       </c>
@@ -8143,7 +8152,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>271</v>
       </c>
@@ -8181,7 +8190,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>272</v>
       </c>
@@ -8219,7 +8228,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>273</v>
       </c>
@@ -8257,7 +8266,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>274</v>
       </c>
@@ -8295,7 +8304,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>275</v>
       </c>
@@ -8333,7 +8342,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>276</v>
       </c>
@@ -8371,7 +8380,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>277</v>
       </c>
@@ -8407,6 +8416,158 @@
       </c>
       <c r="L189" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="190" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
+        <v>278</v>
+      </c>
+      <c r="B190" t="s">
+        <v>13</v>
+      </c>
+      <c r="C190" t="s">
+        <v>14</v>
+      </c>
+      <c r="D190" t="s">
+        <v>29</v>
+      </c>
+      <c r="E190" t="s">
+        <v>16</v>
+      </c>
+      <c r="F190" t="s">
+        <v>17</v>
+      </c>
+      <c r="G190" t="s">
+        <v>30</v>
+      </c>
+      <c r="H190" t="s">
+        <v>19</v>
+      </c>
+      <c r="I190" t="s">
+        <v>19</v>
+      </c>
+      <c r="J190" t="s">
+        <v>83</v>
+      </c>
+      <c r="K190" t="s">
+        <v>84</v>
+      </c>
+      <c r="L190" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="191" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>104</v>
+      </c>
+      <c r="B191" t="s">
+        <v>13</v>
+      </c>
+      <c r="C191" t="s">
+        <v>14</v>
+      </c>
+      <c r="D191" t="s">
+        <v>43</v>
+      </c>
+      <c r="E191" t="s">
+        <v>16</v>
+      </c>
+      <c r="F191" t="s">
+        <v>17</v>
+      </c>
+      <c r="G191" t="s">
+        <v>63</v>
+      </c>
+      <c r="H191" t="s">
+        <v>19</v>
+      </c>
+      <c r="I191" t="s">
+        <v>19</v>
+      </c>
+      <c r="J191" t="s">
+        <v>44</v>
+      </c>
+      <c r="K191" t="s">
+        <v>84</v>
+      </c>
+      <c r="L191" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="192" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>279</v>
+      </c>
+      <c r="B192" t="s">
+        <v>13</v>
+      </c>
+      <c r="C192" t="s">
+        <v>14</v>
+      </c>
+      <c r="D192" t="s">
+        <v>43</v>
+      </c>
+      <c r="E192" t="s">
+        <v>15</v>
+      </c>
+      <c r="F192" t="s">
+        <v>17</v>
+      </c>
+      <c r="G192" t="s">
+        <v>37</v>
+      </c>
+      <c r="H192" t="s">
+        <v>19</v>
+      </c>
+      <c r="I192" t="s">
+        <v>19</v>
+      </c>
+      <c r="J192" t="s">
+        <v>85</v>
+      </c>
+      <c r="K192" t="s">
+        <v>96</v>
+      </c>
+      <c r="L192" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="193" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>280</v>
+      </c>
+      <c r="B193" t="s">
+        <v>13</v>
+      </c>
+      <c r="C193" t="s">
+        <v>14</v>
+      </c>
+      <c r="D193" t="s">
+        <v>43</v>
+      </c>
+      <c r="E193" t="s">
+        <v>16</v>
+      </c>
+      <c r="F193" t="s">
+        <v>17</v>
+      </c>
+      <c r="G193" t="s">
+        <v>18</v>
+      </c>
+      <c r="H193" t="s">
+        <v>19</v>
+      </c>
+      <c r="I193" t="s">
+        <v>19</v>
+      </c>
+      <c r="J193" t="s">
+        <v>21</v>
+      </c>
+      <c r="K193" t="s">
+        <v>21</v>
+      </c>
+      <c r="L193" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>